<commit_message>
feat: add baseline summary
</commit_message>
<xml_diff>
--- a/tests/analysis/case/analysis-ec.test-cases.xlsx
+++ b/tests/analysis/case/analysis-ec.test-cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/cfp-calc/tests/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naoto/Documents/projects/code-for-japan/cfp-calc/tests/analysis/case/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04F4CCD-7583-E446-BA3D-88547B896673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D646E413-069C-354E-971B-01F39F0FDA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="4800" windowWidth="38400" windowHeight="24000" activeTab="3" xr2:uid="{1C382EEA-7345-1D4C-9257-EF0DB7B0E560}"/>
   </bookViews>
@@ -18,10 +18,11 @@
     <sheet name="estimation answer" sheetId="3" r:id="rId3"/>
     <sheet name="housing01" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
-    <pivotCache cacheId="7" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="4" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="117">
   <si>
     <t>水道</t>
     <rPh sb="0" eb="2">
@@ -900,6 +901,10 @@
   </si>
   <si>
     <t>質問票シートで算出した「電力のGHG原単位」</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1310,7 +1315,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1355,15 +1360,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1384,9 +1380,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1414,6 +1407,19 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="パーセント" xfId="1" builtinId="5"/>
@@ -1532,6 +1538,50 @@
         <n v="2.0457431162485458"/>
         <n v="60.521353381165724"/>
       </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45059.823671759259" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10" xr:uid="{C2F4D70A-FFA5-B249-B00B-16D3A870F634}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A36:H46" sheet="housing01"/>
+  </cacheSource>
+  <cacheFields count="8">
+    <cacheField name="domain" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="item" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="subdomain" numFmtId="0">
+      <sharedItems count="4">
+        <s v="construction-maintenance"/>
+        <s v="electricity"/>
+        <s v="other-energy"/>
+        <s v="water"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="value" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.9614220396155515" maxValue="2156.2688418548719"/>
+    </cacheField>
+    <cacheField name="unit" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="value2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.7319211581766772E-2" maxValue="3.4180806918018205"/>
+    </cacheField>
+    <cacheField name="unit2" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="footprint" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.0638487186150329" maxValue="1367.7640445322979"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1752,8 +1802,113 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="10">
+  <r>
+    <s v="housing"/>
+    <s v="imputed-rent"/>
+    <x v="0"/>
+    <n v="32.061793136718038"/>
+    <s v="km-passenger"/>
+    <n v="0.93069899951528912"/>
+    <s v="vehicle"/>
+    <n v="29.839878795009639"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="rent"/>
+    <x v="0"/>
+    <n v="6.9343286819734553"/>
+    <s v="km-passenger"/>
+    <n v="3.4180806918018205"/>
+    <s v="vehicle"/>
+    <n v="23.702094978461034"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="land-rent"/>
+    <x v="0"/>
+    <n v="1.9614220396155515"/>
+    <s v="km-passenger"/>
+    <n v="0.54238644061711094"/>
+    <s v="use"/>
+    <n v="1.0638487186150329"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="housing-maintenance"/>
+    <x v="0"/>
+    <n v="44.183052171363663"/>
+    <s v="km-passenger"/>
+    <n v="1.3782452040258706"/>
+    <s v="000JPY"/>
+    <n v="60.895079754406794"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="electricity"/>
+    <x v="1"/>
+    <n v="2156.2688418548719"/>
+    <s v="km-passenger"/>
+    <n v="0.63431981113992997"/>
+    <s v="000JPY"/>
+    <n v="1367.7640445322979"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="urban-gas"/>
+    <x v="2"/>
+    <n v="886.80383440208766"/>
+    <s v="km-passenger"/>
+    <n v="0.3105447626180039"/>
+    <s v="000JPY"/>
+    <n v="275.39228624313193"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="lpg"/>
+    <x v="2"/>
+    <n v="438.75753482740384"/>
+    <s v="km-passenger"/>
+    <n v="0.32756490664331728"/>
+    <s v="km-passenger"/>
+    <n v="143.72157093479058"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="kerosene"/>
+    <x v="2"/>
+    <n v="650.75993023591275"/>
+    <s v="km-passenger"/>
+    <n v="0.28008110814182374"/>
+    <s v="km-passenger"/>
+    <n v="182.26556239477034"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="other-energy"/>
+    <x v="2"/>
+    <n v="54.817425919256138"/>
+    <s v="km-passenger"/>
+    <n v="3.7319211581766772E-2"/>
+    <s v="km-passenger"/>
+    <n v="2.0457431162485458"/>
+  </r>
+  <r>
+    <s v="housing"/>
+    <s v="water"/>
+    <x v="3"/>
+    <n v="103.55050000000001"/>
+    <s v="km-passenger"/>
+    <n v="0.58446220328405674"/>
+    <s v="km-passenger"/>
+    <n v="60.521353381165724"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8C6C0581-89B5-3344-A4A1-C2F04D43E6F9}" name="ピボットテーブル1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8C6C0581-89B5-3344-A4A1-C2F04D43E6F9}" name="ピボットテーブル1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J25:K30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -1826,7 +1981,66 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4B0CB0C5-1745-6B41-884A-2E54713D838B}" name="ピボットテーブル2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6EE996BA-7685-B148-9FCF-1656D286D1BD}" name="ピボットテーブル1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="J36:K41" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="合計 / footprint" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4B0CB0C5-1745-6B41-884A-2E54713D838B}" name="ピボットテーブル2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="値" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J23:K28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -2212,258 +2426,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="45">
         <v>2</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="50"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="51"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="51"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="47">
         <v>750</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="51"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="51"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="47">
         <v>15</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="51"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="51"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="51" t="b">
+      <c r="D11" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="51"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="47">
         <v>200</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="51"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="47">
         <v>2</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="51"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="52"/>
+      <c r="F14" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -2500,44 +2714,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="37"/>
-      <c r="N1" s="36"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="57"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="21" t="s">
@@ -3330,7 +3544,7 @@
       <c r="N21" s="1"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="J25" s="44" t="s">
+      <c r="J25" s="41" t="s">
         <v>68</v>
       </c>
       <c r="K25" t="s">
@@ -3338,34 +3552,34 @@
       </c>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="42" t="s">
+      <c r="E26" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="42" t="s">
+      <c r="F26" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H26" s="43" t="s">
+      <c r="H26" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="J26" s="45" t="s">
+      <c r="J26" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="K26" s="46">
+      <c r="K26">
         <v>52.149329471594179</v>
       </c>
     </row>
@@ -3395,10 +3609,10 @@
         <f>D27*F27</f>
         <v>11.47801783998437</v>
       </c>
-      <c r="J27" s="45" t="s">
+      <c r="J27" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K27" s="46">
+      <c r="K27">
         <v>2326.430112294016</v>
       </c>
     </row>
@@ -3428,10 +3642,10 @@
         <f t="shared" ref="H28:H36" si="0">D28*F28</f>
         <v>9.1170969854367243</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="K28" s="46">
+      <c r="K28">
         <v>511.31844618440402</v>
       </c>
     </row>
@@ -3461,10 +3675,10 @@
         <f t="shared" si="0"/>
         <v>1.0638487186150329</v>
       </c>
-      <c r="J29" s="45" t="s">
+      <c r="J29" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="K29" s="46">
+      <c r="K29">
         <v>60.521353381165724</v>
       </c>
     </row>
@@ -3494,10 +3708,10 @@
         <f t="shared" si="0"/>
         <v>30.490365927558052</v>
       </c>
-      <c r="J30" s="45" t="s">
+      <c r="J30" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="K30" s="46">
+      <c r="K30">
         <v>2950.4192413311798</v>
       </c>
     </row>
@@ -3897,258 +4111,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="44" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="49">
+      <c r="D2" s="45">
         <v>1</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="50"/>
+      <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="51"/>
+      <c r="F3" s="47"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="51"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="47">
         <v>750</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="47"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="51"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="51" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="51"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="51" t="s">
+      <c r="E8" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="47">
         <v>15</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="51"/>
+      <c r="F9" s="47"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="51"/>
+      <c r="F10" s="47"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="51" t="s">
+      <c r="A11" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="51" t="b">
+      <c r="D11" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="51"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="47">
         <v>200</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="51"/>
+      <c r="F12" s="47"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="47">
         <v>2</v>
       </c>
-      <c r="E13" s="51" t="s">
+      <c r="E13" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="51"/>
+      <c r="F13" s="47"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="52"/>
+      <c r="F14" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -4161,10 +4375,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4185,40 +4399,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="I1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="49" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4256,7 +4470,7 @@
       <c r="K2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="54" t="s">
+      <c r="L2" s="50" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4294,7 +4508,7 @@
       <c r="K3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="55" t="s">
+      <c r="L3" s="51" t="s">
         <v>107</v>
       </c>
     </row>
@@ -4332,7 +4546,7 @@
       <c r="K4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="55" t="s">
+      <c r="L4" s="51" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4370,7 +4584,7 @@
       <c r="K5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="51" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4408,7 +4622,7 @@
       <c r="K6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="56" t="s">
+      <c r="L6" s="52" t="s">
         <v>110</v>
       </c>
     </row>
@@ -4446,7 +4660,7 @@
       <c r="K7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="55" t="s">
+      <c r="L7" s="51" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4484,7 +4698,7 @@
       <c r="K8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="55" t="s">
+      <c r="L8" s="51" t="s">
         <v>112</v>
       </c>
     </row>
@@ -4522,7 +4736,7 @@
       <c r="K9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="55" t="s">
+      <c r="L9" s="51" t="s">
         <v>113</v>
       </c>
     </row>
@@ -4560,7 +4774,7 @@
       <c r="K10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="55" t="s">
+      <c r="L10" s="51" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4598,7 +4812,7 @@
       <c r="K11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="53" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4636,7 +4850,7 @@
       <c r="K12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="55"/>
+      <c r="L12" s="51"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="12" t="s">
@@ -4672,7 +4886,7 @@
       <c r="K13" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L13" s="55"/>
+      <c r="L13" s="51"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="12" t="s">
@@ -4708,7 +4922,7 @@
       <c r="K14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="55"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="12" t="s">
@@ -4744,7 +4958,7 @@
       <c r="K15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="55"/>
+      <c r="L15" s="51"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="12" t="s">
@@ -4780,7 +4994,7 @@
       <c r="K16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="55" t="s">
+      <c r="L16" s="51" t="s">
         <v>115</v>
       </c>
     </row>
@@ -4818,7 +5032,7 @@
       <c r="K17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="55"/>
+      <c r="L17" s="51"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="12" t="s">
@@ -4854,7 +5068,7 @@
       <c r="K18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L18" s="55"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="12" t="s">
@@ -4890,7 +5104,7 @@
       <c r="K19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L19" s="55"/>
+      <c r="L19" s="51"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="12" t="s">
@@ -4926,7 +5140,7 @@
       <c r="K20" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="55"/>
+      <c r="L20" s="51"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
@@ -4962,34 +5176,34 @@
       <c r="K21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L21" s="57"/>
+      <c r="L21" s="53"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="42" t="s">
+      <c r="E23" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="42" t="s">
+      <c r="F23" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="43" t="s">
+      <c r="H23" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="41" t="s">
         <v>68</v>
       </c>
       <c r="K23" t="s">
@@ -5018,14 +5232,14 @@
       <c r="G24" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="58">
+      <c r="H24" s="54">
         <f>D24*F24</f>
         <v>15.304023786645827</v>
       </c>
-      <c r="J24" s="45" t="s">
+      <c r="J24" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="46">
+      <c r="K24">
         <v>59.755353509753476</v>
       </c>
     </row>
@@ -5055,10 +5269,10 @@
         <f t="shared" ref="H25:H33" si="0">D25*F25</f>
         <v>12.156129313915635</v>
       </c>
-      <c r="J25" s="45" t="s">
+      <c r="J25" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="46">
+      <c r="K25">
         <v>4355.5720706511465</v>
       </c>
     </row>
@@ -5088,10 +5302,10 @@
         <f t="shared" si="0"/>
         <v>1.0638487186150329</v>
       </c>
-      <c r="J26" s="45" t="s">
+      <c r="J26" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="K26" s="46">
+      <c r="K26">
         <v>1499.8507462997977</v>
       </c>
     </row>
@@ -5121,10 +5335,10 @@
         <f t="shared" si="0"/>
         <v>31.231351690576975</v>
       </c>
-      <c r="J27" s="45" t="s">
+      <c r="J27" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="K27" s="46">
+      <c r="K27">
         <v>60.521353381165724</v>
       </c>
     </row>
@@ -5154,10 +5368,10 @@
         <f t="shared" si="0"/>
         <v>4355.5720706511438</v>
       </c>
-      <c r="J28" s="45" t="s">
+      <c r="J28" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="K28" s="46">
+      <c r="K28">
         <v>5975.6995238418631</v>
       </c>
     </row>
@@ -5269,7 +5483,7 @@
         <v>2.0457431162485458</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:11">
       <c r="A33" s="2" t="s">
         <v>7</v>
       </c>
@@ -5293,6 +5507,343 @@
       </c>
       <c r="H33" s="3">
         <f t="shared" si="0"/>
+        <v>60.521353381165724</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="21">
+        <v>32.061793136718038</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0.93069899951528912</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H37" s="54">
+        <f>D37*F37</f>
+        <v>29.839878795009639</v>
+      </c>
+      <c r="J37" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="K37" s="59">
+        <v>115.5009022464925</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="12">
+        <v>6.9343286819734553</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="12">
+        <v>3.4180806918018205</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H38" s="16">
+        <f t="shared" ref="H38:H46" si="1">D38*F38</f>
+        <v>23.702094978461034</v>
+      </c>
+      <c r="J38" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="59">
+        <v>1367.7640445322979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1.9614220396155515</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0.54238644061711094</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H39" s="16">
+        <f t="shared" si="1"/>
+        <v>1.0638487186150329</v>
+      </c>
+      <c r="J39" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K39" s="59">
+        <v>603.42516268894144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="12">
+        <v>44.183052171363663</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="12">
+        <v>1.3782452040258706</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="16">
+        <f t="shared" si="1"/>
+        <v>60.895079754406794</v>
+      </c>
+      <c r="J40" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" s="59">
+        <v>60.521353381165724</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="12">
+        <v>2156.2688418548701</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0.63431981113992997</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="16">
+        <f t="shared" si="1"/>
+        <v>1367.7640445322968</v>
+      </c>
+      <c r="J41" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="59">
+        <v>2147.2114628488976</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="12">
+        <v>886.80383440208766</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0.3105447626180039</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="16">
+        <f t="shared" si="1"/>
+        <v>275.39228624313193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="12">
+        <v>438.75753482740384</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0.32756490664331728</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H43" s="16">
+        <f t="shared" si="1"/>
+        <v>143.72157093479058</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="12">
+        <v>650.75993023591275</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0.28008110814182374</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="16">
+        <f t="shared" si="1"/>
+        <v>182.26556239477034</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="12">
+        <v>54.817425919256138</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="12">
+        <v>3.7319211581766772E-2</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" s="16">
+        <f t="shared" si="1"/>
+        <v>2.0457431162485458</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2">
+        <v>103.55050000000001</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.58446220328405674</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H46" s="3">
+        <f t="shared" si="1"/>
         <v>60.521353381165724</v>
       </c>
     </row>

</xml_diff>